<commit_message>
added settings, password change and account deletion
</commit_message>
<xml_diff>
--- a/cypress/testupload.xlsx
+++ b/cypress/testupload.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DFE71D-215B-4198-9E9E-264FCCA74215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074C3913-FF6F-4631-88B6-A325C627F77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14415" yWindow="4080" windowWidth="21600" windowHeight="11385" xr2:uid="{68530765-9C47-4B1A-B2BC-08AEA67A5497}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{68530765-9C47-4B1A-B2BC-08AEA67A5497}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>name</t>
   </si>
@@ -54,9 +54,6 @@
     <t>positiontitle</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>Developer</t>
   </si>
   <si>
-    <t>testingh</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -99,13 +93,34 @@
     <t>interviewing</t>
   </si>
   <si>
-    <t>"Java, Python"</t>
-  </si>
-  <si>
-    <t>test@gmail.com</t>
-  </si>
-  <si>
-    <t>hhfdfgh@gmail.com</t>
+    <t>Eric Bradshaw</t>
+  </si>
+  <si>
+    <t>Eric Wong</t>
+  </si>
+  <si>
+    <t>Eliass Ghauss</t>
+  </si>
+  <si>
+    <t>ericbradshaw@gmail.com</t>
+  </si>
+  <si>
+    <t>ericwong@gmail.com</t>
+  </si>
+  <si>
+    <t>eliassghauss@gmail.com</t>
+  </si>
+  <si>
+    <t>teacher</t>
+  </si>
+  <si>
+    <t>employee</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>Hiring Manager</t>
   </si>
 </sst>
 </file>
@@ -477,13 +492,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A05D0592-5A20-4292-B8DC-08604C6DADA8}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -496,7 +515,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -511,22 +530,22 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" t="s">
         <v>20</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>21</v>
       </c>
-      <c r="L1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" t="s">
-        <v>23</v>
-      </c>
       <c r="N1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O1" t="s">
         <v>7</v>
@@ -537,34 +556,34 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -578,43 +597,41 @@
       <c r="N2">
         <v>0</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="O2" s="1"/>
       <c r="P2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -628,19 +645,64 @@
       <c r="N3">
         <v>0</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="P3" t="s">
-        <v>14</v>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="P4" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{7687C314-E90B-458F-8E98-5A7627BC7732}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{A81C5A11-0A4B-4FAD-9878-D84B0AE5BCA7}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{146D5112-2297-4BD1-AFF6-3E81E9C88A48}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>